<commit_message>
Gastos del Fin de semana
</commit_message>
<xml_diff>
--- a/Finanzas/1_Ene-Feb-Mar_2018.xlsx
+++ b/Finanzas/1_Ene-Feb-Mar_2018.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro\Desktop\Felisa\Finanzas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adriana\Desktop\Felisa\Finanzas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="154">
   <si>
     <t>E L             D I N E R O         E  S             U N             R E C U R S O      L I M I T A D O</t>
   </si>
@@ -459,6 +459,33 @@
   </si>
   <si>
     <t>Cuatrimestre</t>
+  </si>
+  <si>
+    <t>Jaime</t>
+  </si>
+  <si>
+    <t>Prestamo 1</t>
+  </si>
+  <si>
+    <t>Escuela Manejo</t>
+  </si>
+  <si>
+    <t>Paletas Carlos V</t>
+  </si>
+  <si>
+    <t>Gnomo</t>
+  </si>
+  <si>
+    <t>Fondita Condesa</t>
+  </si>
+  <si>
+    <t>Estacionamiento Samborns</t>
+  </si>
+  <si>
+    <t>Sukiya</t>
+  </si>
+  <si>
+    <t>Tiendita</t>
   </si>
 </sst>
 </file>
@@ -1323,8 +1350,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BH963"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1602,7 +1629,7 @@
       </c>
       <c r="P4" s="79">
         <f>SUM(N3,R9,P7)</f>
-        <v>38074</v>
+        <v>40832</v>
       </c>
       <c r="Z4" s="47">
         <v>43108</v>
@@ -1675,7 +1702,7 @@
       </c>
       <c r="BG4" s="57">
         <f>(SUM((AV3:AV519)))-(SUM((AZ3:AZ519)))</f>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="BH4" s="57"/>
     </row>
@@ -1781,7 +1808,7 @@
       </c>
       <c r="N6" s="52">
         <f>(SUM((W11:W299),(AC3:AC500),(I11:I499)))-(SUM((X11:X499)))</f>
-        <v>273</v>
+        <v>531</v>
       </c>
       <c r="O6" s="30"/>
       <c r="P6" s="30"/>
@@ -1868,17 +1895,17 @@
       </c>
       <c r="P7" s="78">
         <f>SUM(R7,N6)</f>
-        <v>273</v>
+        <v>3031</v>
       </c>
       <c r="Q7" s="75"/>
       <c r="R7" s="74">
         <f>(SUM(X11:X499))-(SUM(K11:K499))</f>
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="S7" s="116"/>
       <c r="T7" s="118">
         <f>E9</f>
-        <v>12160</v>
+        <v>10160</v>
       </c>
       <c r="Z7" s="47">
         <v>43111</v>
@@ -2016,7 +2043,7 @@
       <c r="D9" s="61"/>
       <c r="E9" s="44">
         <f>SUM(E10:E500)</f>
-        <v>12160</v>
+        <v>10160</v>
       </c>
       <c r="G9" s="10" t="s">
         <v>16</v>
@@ -2536,17 +2563,26 @@
       <c r="AB13" s="49"/>
       <c r="AC13" s="41">
         <f>(SUM(AD13,AE13))-AG13</f>
-        <v>0</v>
-      </c>
-      <c r="AD13" s="50"/>
+        <v>-6858</v>
+      </c>
+      <c r="AD13" s="50">
+        <v>80</v>
+      </c>
       <c r="AE13" s="50"/>
       <c r="AG13" s="51">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AI13" s="100"/>
+        <v>6938</v>
+      </c>
+      <c r="AH13">
+        <v>70</v>
+      </c>
+      <c r="AI13" s="100" t="s">
+        <v>114</v>
+      </c>
       <c r="AJ13" s="56"/>
-      <c r="AK13" s="56"/>
+      <c r="AK13" s="15">
+        <v>6850</v>
+      </c>
       <c r="AL13" s="56"/>
       <c r="AM13" s="56"/>
       <c r="AN13" s="56"/>
@@ -2558,7 +2594,7 @@
       <c r="AT13" s="56"/>
       <c r="AU13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="AV13" s="56"/>
       <c r="AW13" s="56"/>
@@ -2568,10 +2604,15 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="BA13" s="110"/>
+      <c r="BA13" s="110">
+        <v>2</v>
+      </c>
       <c r="BB13">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="BC13">
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:60" x14ac:dyDescent="0.25">
@@ -2582,11 +2623,11 @@
         <v>141</v>
       </c>
       <c r="C14">
-        <v>10000</v>
+        <v>8000</v>
       </c>
       <c r="E14">
         <f t="shared" si="6"/>
-        <v>10000</v>
+        <v>8000</v>
       </c>
       <c r="G14" s="99">
         <v>43116</v>
@@ -2638,17 +2679,28 @@
       <c r="AB14" s="49"/>
       <c r="AC14" s="41">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AD14" s="50"/>
+        <v>-86</v>
+      </c>
+      <c r="AD14" s="50">
+        <v>80</v>
+      </c>
       <c r="AE14" s="50"/>
       <c r="AG14" s="51">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AI14" s="100"/>
-      <c r="AJ14" s="56"/>
-      <c r="AK14" s="56"/>
+        <v>166</v>
+      </c>
+      <c r="AH14">
+        <v>100</v>
+      </c>
+      <c r="AI14" s="100" t="s">
+        <v>150</v>
+      </c>
+      <c r="AJ14" s="56" t="s">
+        <v>151</v>
+      </c>
+      <c r="AK14" s="56">
+        <v>10</v>
+      </c>
       <c r="AL14" s="56"/>
       <c r="AM14" s="56"/>
       <c r="AN14" s="56"/>
@@ -2660,20 +2712,29 @@
       <c r="AT14" s="56"/>
       <c r="AU14">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AV14" s="56"/>
-      <c r="AW14" s="56"/>
+        <v>56</v>
+      </c>
+      <c r="AV14" s="56">
+        <v>50</v>
+      </c>
+      <c r="AW14" s="56">
+        <v>2</v>
+      </c>
       <c r="AX14" s="56"/>
-      <c r="AY14" s="56"/>
+      <c r="AY14" s="56">
+        <v>1</v>
+      </c>
       <c r="AZ14" s="56">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="BA14" s="56"/>
       <c r="BB14">
         <f t="shared" si="4"/>
         <v>0</v>
+      </c>
+      <c r="BC14">
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:60" x14ac:dyDescent="0.25">
@@ -2709,7 +2770,7 @@
       </c>
       <c r="V15" s="35"/>
       <c r="W15" s="37">
-        <v>100</v>
+        <v>250</v>
       </c>
       <c r="X15" s="37"/>
       <c r="Z15" s="47">
@@ -2721,17 +2782,28 @@
       <c r="AB15" s="72"/>
       <c r="AC15" s="41">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AD15" s="50"/>
+        <v>27</v>
+      </c>
+      <c r="AD15" s="50">
+        <v>80</v>
+      </c>
       <c r="AE15" s="50"/>
       <c r="AG15" s="51">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AI15" s="56"/>
-      <c r="AJ15" s="56"/>
-      <c r="AK15" s="56"/>
+        <v>53</v>
+      </c>
+      <c r="AH15">
+        <v>30</v>
+      </c>
+      <c r="AI15" s="56" t="s">
+        <v>149</v>
+      </c>
+      <c r="AJ15" s="56" t="s">
+        <v>148</v>
+      </c>
+      <c r="AK15" s="56">
+        <v>18</v>
+      </c>
       <c r="AL15" s="56"/>
       <c r="AM15" s="56"/>
       <c r="AN15" s="56"/>
@@ -2743,20 +2815,24 @@
       <c r="AT15" s="56"/>
       <c r="AU15">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AV15" s="56"/>
       <c r="AW15" s="56"/>
       <c r="AX15" s="56"/>
-      <c r="AY15" s="56"/>
+      <c r="AY15" s="56">
+        <v>1</v>
+      </c>
       <c r="AZ15" s="56">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="BA15" s="56"/>
+        <v>5</v>
+      </c>
+      <c r="BA15" s="56">
+        <v>1</v>
+      </c>
       <c r="BB15">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:60" x14ac:dyDescent="0.25">
@@ -2784,10 +2860,18 @@
         <f t="shared" si="5"/>
         <v>120</v>
       </c>
-      <c r="T16" s="35"/>
-      <c r="U16" s="35"/>
-      <c r="V16" s="35"/>
-      <c r="W16" s="37"/>
+      <c r="T16" s="36">
+        <v>43116</v>
+      </c>
+      <c r="U16" s="35" t="s">
+        <v>145</v>
+      </c>
+      <c r="V16" s="35" t="s">
+        <v>146</v>
+      </c>
+      <c r="W16" s="37">
+        <v>8000</v>
+      </c>
       <c r="X16" s="37"/>
       <c r="Z16" s="47">
         <v>43120</v>
@@ -2798,17 +2882,28 @@
       <c r="AB16" s="49"/>
       <c r="AC16" s="41">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AD16" s="50"/>
+        <v>-25</v>
+      </c>
+      <c r="AD16" s="50">
+        <v>100</v>
+      </c>
       <c r="AE16" s="50"/>
       <c r="AG16" s="68">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AI16" s="56"/>
-      <c r="AJ16" s="56"/>
-      <c r="AK16" s="56"/>
+        <v>125</v>
+      </c>
+      <c r="AH16">
+        <v>100</v>
+      </c>
+      <c r="AI16" s="56" t="s">
+        <v>152</v>
+      </c>
+      <c r="AJ16" s="56" t="s">
+        <v>153</v>
+      </c>
+      <c r="AK16" s="56">
+        <v>15</v>
+      </c>
       <c r="AL16" s="56"/>
       <c r="AM16" s="56"/>
       <c r="AN16" s="56"/>
@@ -2820,7 +2915,7 @@
       <c r="AT16" s="56"/>
       <c r="AU16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AV16" s="56"/>
       <c r="AW16" s="56"/>
@@ -2830,10 +2925,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="BA16" s="56"/>
+      <c r="BA16" s="56">
+        <v>2</v>
+      </c>
       <c r="BB16">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="5:60" x14ac:dyDescent="0.25">
@@ -2861,11 +2958,21 @@
         <f t="shared" si="5"/>
         <v>500</v>
       </c>
-      <c r="T17" s="36"/>
-      <c r="U17" s="35"/>
-      <c r="V17" s="35"/>
-      <c r="W17" s="37"/>
-      <c r="X17" s="37"/>
+      <c r="T17" s="36">
+        <v>43119</v>
+      </c>
+      <c r="U17" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="V17" s="35" t="s">
+        <v>147</v>
+      </c>
+      <c r="W17" s="37">
+        <v>1300</v>
+      </c>
+      <c r="X17" s="37">
+        <v>2500</v>
+      </c>
       <c r="Z17" s="47">
         <v>43121</v>
       </c>
@@ -2938,10 +3045,18 @@
         <f t="shared" si="5"/>
         <v>150</v>
       </c>
-      <c r="T18" s="36"/>
-      <c r="U18" s="35"/>
-      <c r="V18" s="35"/>
-      <c r="W18" s="37"/>
+      <c r="T18" s="36">
+        <v>43119</v>
+      </c>
+      <c r="U18" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="V18" s="35" t="s">
+        <v>124</v>
+      </c>
+      <c r="W18" s="37">
+        <v>250</v>
+      </c>
       <c r="X18" s="37"/>
       <c r="Z18" s="47">
         <v>43122</v>

</xml_diff>

<commit_message>
Gastos viernes y sabado
</commit_message>
<xml_diff>
--- a/Finanzas/1_Ene-Feb-Mar_2018.xlsx
+++ b/Finanzas/1_Ene-Feb-Mar_2018.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro\Desktop\Felisa\Finanzas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adriana\Desktop\Felisa\Finanzas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="171">
   <si>
     <t>E L             D I N E R O         E  S             U N             R E C U R S O      L I M I T A D O</t>
   </si>
@@ -523,6 +523,21 @@
   <si>
     <t>Uri y Niño LAB :D</t>
   </si>
+  <si>
+    <t>Houston's</t>
+  </si>
+  <si>
+    <t>Pizza</t>
+  </si>
+  <si>
+    <t>Diente Roto</t>
+  </si>
+  <si>
+    <t>Tío Niño 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avatar FINAL </t>
+  </si>
 </sst>
 </file>
 
@@ -884,7 +899,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1090,6 +1105,7 @@
     <xf numFmtId="0" fontId="21" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="22" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1386,8 +1402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BH963"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1666,7 +1682,7 @@
       </c>
       <c r="P4" s="79">
         <f>SUM(N3,R9,P7)</f>
-        <v>41060</v>
+        <v>40630</v>
       </c>
       <c r="Z4" s="47">
         <v>43108</v>
@@ -1739,7 +1755,7 @@
       </c>
       <c r="BG4" s="57">
         <f>(SUM((AV3:AV519)))-(SUM((AZ3:AZ519)))</f>
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="BH4" s="57"/>
     </row>
@@ -1845,7 +1861,7 @@
       </c>
       <c r="N6" s="52">
         <f>(SUM((W11:W299),(AC3:AC500),(I11:I499)))-(SUM((X11:X499)))</f>
-        <v>159</v>
+        <v>1729</v>
       </c>
       <c r="O6" s="30"/>
       <c r="P6" s="30"/>
@@ -1933,12 +1949,12 @@
       </c>
       <c r="P7" s="78">
         <f>SUM(R7,N6)</f>
-        <v>2159</v>
+        <v>1729</v>
       </c>
       <c r="Q7" s="75"/>
       <c r="R7" s="74">
         <f>(SUM(X11:X499))-(SUM(K11:K499))</f>
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="S7" s="116"/>
       <c r="T7" s="118">
@@ -3025,7 +3041,7 @@
         <v>1300</v>
       </c>
       <c r="X17" s="37">
-        <v>2500</v>
+        <v>1100</v>
       </c>
       <c r="Z17" s="47">
         <v>43121</v>
@@ -3212,11 +3228,9 @@
       </c>
       <c r="V19" s="35"/>
       <c r="W19" s="37">
-        <v>150</v>
-      </c>
-      <c r="X19" s="37">
-        <v>600</v>
-      </c>
+        <v>250</v>
+      </c>
+      <c r="X19" s="37"/>
       <c r="Z19" s="47">
         <v>43123</v>
       </c>
@@ -3400,7 +3414,7 @@
       </c>
       <c r="AC21" s="41">
         <f t="shared" si="3"/>
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="AD21" s="50">
         <v>80</v>
@@ -3408,9 +3422,12 @@
       <c r="AE21" s="70"/>
       <c r="AG21" s="51">
         <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="AI21" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="AH21">
+        <v>70</v>
+      </c>
+      <c r="AI21" s="100" t="s">
         <v>114</v>
       </c>
       <c r="AJ21" s="100"/>
@@ -3429,12 +3446,16 @@
         <v>10</v>
       </c>
       <c r="AV21" s="56"/>
-      <c r="AW21" s="56"/>
+      <c r="AW21" s="56">
+        <v>1</v>
+      </c>
       <c r="AX21" s="56"/>
-      <c r="AY21" s="109"/>
+      <c r="AY21" s="109">
+        <v>2</v>
+      </c>
       <c r="AZ21" s="56">
         <f t="shared" ref="AZ21:AZ84" si="7">(AW21*6)+(AX21*8)+(AY21*5)</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="BA21" s="56">
         <v>2</v>
@@ -3480,20 +3501,33 @@
       <c r="AA22" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="AB22" s="49"/>
+      <c r="AB22" s="49" t="s">
+        <v>169</v>
+      </c>
       <c r="AC22" s="41">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AD22" s="67"/>
+        <v>-450</v>
+      </c>
+      <c r="AD22" s="67">
+        <v>80</v>
+      </c>
       <c r="AE22" s="67"/>
       <c r="AG22" s="51">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AI22" s="56"/>
-      <c r="AJ22" s="56"/>
-      <c r="AK22" s="56"/>
+        <v>530</v>
+      </c>
+      <c r="AH22">
+        <v>100</v>
+      </c>
+      <c r="AI22" s="56" t="s">
+        <v>166</v>
+      </c>
+      <c r="AJ22" s="56" t="s">
+        <v>168</v>
+      </c>
+      <c r="AK22" s="56">
+        <v>400</v>
+      </c>
       <c r="AL22" s="56"/>
       <c r="AM22" s="56"/>
       <c r="AN22" s="56"/>
@@ -3505,20 +3539,28 @@
       <c r="AT22" s="56"/>
       <c r="AU22">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AV22" s="56"/>
-      <c r="AW22" s="56"/>
+        <v>30</v>
+      </c>
+      <c r="AV22" s="56">
+        <v>20</v>
+      </c>
+      <c r="AW22" s="56">
+        <v>2</v>
+      </c>
       <c r="AX22" s="56"/>
-      <c r="AY22" s="56"/>
+      <c r="AY22" s="56">
+        <v>2</v>
+      </c>
       <c r="AZ22" s="56">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="BA22" s="56"/>
+        <v>22</v>
+      </c>
+      <c r="BA22" s="56">
+        <v>2</v>
+      </c>
       <c r="BB22">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:60" x14ac:dyDescent="0.25">
@@ -3558,20 +3600,33 @@
       <c r="AA23" s="48" t="s">
         <v>70</v>
       </c>
-      <c r="AB23" s="49"/>
+      <c r="AB23" s="49" t="s">
+        <v>170</v>
+      </c>
       <c r="AC23" s="41">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AD23" s="50"/>
+        <v>-10</v>
+      </c>
+      <c r="AD23" s="50">
+        <v>100</v>
+      </c>
       <c r="AE23" s="50"/>
       <c r="AG23" s="51">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AI23" s="56"/>
-      <c r="AJ23" s="56"/>
-      <c r="AK23" s="56"/>
+        <v>110</v>
+      </c>
+      <c r="AH23">
+        <v>100</v>
+      </c>
+      <c r="AI23" s="56" t="s">
+        <v>167</v>
+      </c>
+      <c r="AJ23" s="56" t="s">
+        <v>83</v>
+      </c>
+      <c r="AK23" s="56">
+        <v>10</v>
+      </c>
       <c r="AL23" s="109"/>
       <c r="AM23" s="56"/>
       <c r="AN23" s="56"/>
@@ -3588,10 +3643,12 @@
       <c r="AV23" s="56"/>
       <c r="AW23" s="56"/>
       <c r="AX23" s="56"/>
-      <c r="AY23" s="56"/>
+      <c r="AY23" s="56">
+        <v>2</v>
+      </c>
       <c r="AZ23" s="56">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="BA23" s="56"/>
       <c r="BB23">
@@ -3637,7 +3694,7 @@
       <c r="AA24" s="48" t="s">
         <v>71</v>
       </c>
-      <c r="AB24" s="49"/>
+      <c r="AB24" s="121"/>
       <c r="AC24" s="41">
         <f t="shared" si="3"/>
         <v>0</v>

</xml_diff>

<commit_message>
Fin de semana largo
</commit_message>
<xml_diff>
--- a/Finanzas/1_Ene-Feb-Mar_2018.xlsx
+++ b/Finanzas/1_Ene-Feb-Mar_2018.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro\Desktop\Felisa\Finanzas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adriana\Desktop\Felisa\Finanzas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="187">
   <si>
     <t>E L             D I N E R O         E  S             U N             R E C U R S O      L I M I T A D O</t>
   </si>
@@ -558,6 +558,33 @@
   </si>
   <si>
     <t>Doc Luz Verde</t>
+  </si>
+  <si>
+    <t>Tarjeta Jaime</t>
+  </si>
+  <si>
+    <t>Antihistamínico</t>
+  </si>
+  <si>
+    <t>El Pescadito</t>
+  </si>
+  <si>
+    <t>Hooters</t>
+  </si>
+  <si>
+    <t>Tamales con Jaime</t>
+  </si>
+  <si>
+    <t>Jaime Pescadito Alergia</t>
+  </si>
+  <si>
+    <t>Bautizo Leo</t>
+  </si>
+  <si>
+    <t>Tamales Abuelita Jaime</t>
+  </si>
+  <si>
+    <t>Edgar!!!!</t>
   </si>
 </sst>
 </file>
@@ -1424,7 +1451,7 @@
   <dimension ref="A1:BH963"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1703,7 +1730,7 @@
       </c>
       <c r="P4" s="79">
         <f>SUM(N3,R9,P7)</f>
-        <v>43341</v>
+        <v>43131</v>
       </c>
       <c r="Z4" s="47">
         <v>43108</v>
@@ -1882,7 +1909,7 @@
       </c>
       <c r="N6" s="52">
         <f>(SUM((W11:W299),(AC3:AC500),(I11:I499)))-(SUM((X11:X499)))</f>
-        <v>1440</v>
+        <v>1230</v>
       </c>
       <c r="O6" s="30"/>
       <c r="P6" s="30"/>
@@ -1970,7 +1997,7 @@
       </c>
       <c r="P7" s="78">
         <f>SUM(R7,N6)</f>
-        <v>1440</v>
+        <v>1230</v>
       </c>
       <c r="Q7" s="75"/>
       <c r="R7" s="74">
@@ -3426,8 +3453,12 @@
         <f t="shared" si="5"/>
         <v>300</v>
       </c>
-      <c r="T21" s="36"/>
-      <c r="U21" s="35"/>
+      <c r="T21" s="36">
+        <v>43131</v>
+      </c>
+      <c r="U21" s="35" t="s">
+        <v>186</v>
+      </c>
       <c r="V21" s="35"/>
       <c r="W21" s="37">
         <v>3000</v>
@@ -4186,7 +4217,7 @@
       </c>
       <c r="AC29" s="69">
         <f t="shared" si="3"/>
-        <v>-525</v>
+        <v>-675</v>
       </c>
       <c r="AD29" s="50">
         <v>80</v>
@@ -4194,9 +4225,14 @@
       <c r="AE29" s="84"/>
       <c r="AG29" s="51">
         <f t="shared" si="0"/>
-        <v>605</v>
-      </c>
-      <c r="AI29" s="56"/>
+        <v>755</v>
+      </c>
+      <c r="AH29">
+        <v>150</v>
+      </c>
+      <c r="AI29" s="56" t="s">
+        <v>181</v>
+      </c>
       <c r="AJ29" s="56"/>
       <c r="AK29" s="56"/>
       <c r="AL29" s="56">
@@ -4270,20 +4306,33 @@
       <c r="AA30" s="48" t="s">
         <v>70</v>
       </c>
-      <c r="AB30" s="49"/>
+      <c r="AB30" s="49" t="s">
+        <v>185</v>
+      </c>
       <c r="AC30" s="41">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AD30" s="50"/>
+        <v>-30</v>
+      </c>
+      <c r="AD30" s="50">
+        <v>120</v>
+      </c>
       <c r="AE30" s="50"/>
       <c r="AG30" s="51">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AI30" s="56"/>
-      <c r="AJ30" s="56"/>
-      <c r="AK30" s="56"/>
+        <v>150</v>
+      </c>
+      <c r="AH30">
+        <v>120</v>
+      </c>
+      <c r="AI30" s="56" t="s">
+        <v>182</v>
+      </c>
+      <c r="AJ30" s="56" t="s">
+        <v>178</v>
+      </c>
+      <c r="AK30" s="56">
+        <v>20</v>
+      </c>
       <c r="AL30" s="56"/>
       <c r="AM30" s="56"/>
       <c r="AN30" s="56"/>
@@ -4295,7 +4344,7 @@
       <c r="AT30" s="56"/>
       <c r="AU30">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AV30" s="95"/>
       <c r="AW30" s="56"/>
@@ -4305,10 +4354,12 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="BA30" s="56"/>
+      <c r="BA30" s="56">
+        <v>2</v>
+      </c>
       <c r="BB30">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:60" x14ac:dyDescent="0.25">
@@ -4347,7 +4398,9 @@
       <c r="AA31" s="48" t="s">
         <v>71</v>
       </c>
-      <c r="AB31" s="49"/>
+      <c r="AB31" s="49" t="s">
+        <v>184</v>
+      </c>
       <c r="AC31" s="41">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4424,21 +4477,33 @@
       <c r="AA32" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="AB32" s="49"/>
+      <c r="AB32" s="49" t="s">
+        <v>183</v>
+      </c>
       <c r="AC32" s="41">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AD32" s="50"/>
+        <v>-30</v>
+      </c>
+      <c r="AD32" s="50">
+        <v>100</v>
+      </c>
       <c r="AE32" s="50"/>
       <c r="AG32" s="51">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AH32" s="71"/>
-      <c r="AI32" s="56"/>
-      <c r="AJ32" s="56"/>
-      <c r="AK32" s="56"/>
+        <v>130</v>
+      </c>
+      <c r="AH32" s="71">
+        <v>100</v>
+      </c>
+      <c r="AI32" s="56" t="s">
+        <v>180</v>
+      </c>
+      <c r="AJ32" s="56" t="s">
+        <v>179</v>
+      </c>
+      <c r="AK32" s="56">
+        <v>20</v>
+      </c>
       <c r="AL32" s="56"/>
       <c r="AM32" s="56"/>
       <c r="AN32" s="56"/>
@@ -4450,7 +4515,7 @@
       <c r="AT32" s="56"/>
       <c r="AU32">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AV32" s="56"/>
       <c r="AW32" s="56"/>
@@ -4460,10 +4525,12 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="BA32" s="56"/>
+      <c r="BA32" s="56">
+        <v>2</v>
+      </c>
       <c r="BB32">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="5:56" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Descripción de las Figuras
</commit_message>
<xml_diff>
--- a/Finanzas/1_Ene-Feb-Mar_2018.xlsx
+++ b/Finanzas/1_Ene-Feb-Mar_2018.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="194">
   <si>
     <t>E L             D I N E R O         E  S             U N             R E C U R S O      L I M I T A D O</t>
   </si>
@@ -603,6 +603,9 @@
   </si>
   <si>
     <t>Depto Jaime</t>
+  </si>
+  <si>
+    <t>Dentista Muela 1</t>
   </si>
 </sst>
 </file>
@@ -1469,7 +1472,7 @@
   <dimension ref="A1:BH963"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1748,7 +1751,7 @@
       </c>
       <c r="P4" s="79">
         <f>SUM(N3,R9,P7)</f>
-        <v>42348</v>
+        <v>41916</v>
       </c>
       <c r="Z4" s="47">
         <v>43108</v>
@@ -1821,7 +1824,7 @@
       </c>
       <c r="BG4" s="57">
         <f>(SUM((AV3:AV519)))-(SUM((AZ3:AZ519)))</f>
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="BH4" s="57"/>
     </row>
@@ -1927,7 +1930,7 @@
       </c>
       <c r="N6" s="52">
         <f>(SUM((W11:W299),(AC3:AC500),(I11:I499)))-(SUM((X11:X499)))</f>
-        <v>947</v>
+        <v>515</v>
       </c>
       <c r="O6" s="30"/>
       <c r="P6" s="30"/>
@@ -2015,7 +2018,7 @@
       </c>
       <c r="P7" s="78">
         <f>SUM(R7,N6)</f>
-        <v>947</v>
+        <v>515</v>
       </c>
       <c r="Q7" s="75"/>
       <c r="R7" s="74">
@@ -3683,7 +3686,7 @@
       </c>
       <c r="V23" s="35"/>
       <c r="W23" s="37">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="X23" s="37"/>
       <c r="Y23" s="73"/>
@@ -4788,7 +4791,7 @@
       </c>
       <c r="AC35" s="41">
         <f t="shared" si="3"/>
-        <v>74</v>
+        <v>24</v>
       </c>
       <c r="AD35" s="50">
         <v>80</v>
@@ -4796,7 +4799,10 @@
       <c r="AE35" s="50"/>
       <c r="AG35" s="51">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>56</v>
+      </c>
+      <c r="AH35">
+        <v>50</v>
       </c>
       <c r="AI35" s="56"/>
       <c r="AJ35" s="56"/>
@@ -4865,20 +4871,28 @@
       <c r="AA36" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="AB36" s="49"/>
+      <c r="AB36" s="49" t="s">
+        <v>193</v>
+      </c>
       <c r="AC36" s="41">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AD36" s="50"/>
+        <v>-432</v>
+      </c>
+      <c r="AD36" s="50">
+        <v>80</v>
+      </c>
       <c r="AE36" s="50"/>
       <c r="AG36" s="51">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>512</v>
       </c>
       <c r="AI36" s="56"/>
-      <c r="AJ36" s="56"/>
-      <c r="AK36" s="56"/>
+      <c r="AJ36" s="56" t="s">
+        <v>193</v>
+      </c>
+      <c r="AK36" s="56">
+        <v>500</v>
+      </c>
       <c r="AL36" s="56"/>
       <c r="AM36" s="56"/>
       <c r="AN36" s="56"/>
@@ -4890,15 +4904,21 @@
       <c r="AT36" s="56"/>
       <c r="AU36">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AV36" s="56"/>
-      <c r="AW36" s="56"/>
+        <v>12</v>
+      </c>
+      <c r="AV36" s="56">
+        <v>12</v>
+      </c>
+      <c r="AW36" s="56">
+        <v>2</v>
+      </c>
       <c r="AX36" s="56"/>
-      <c r="AY36" s="56"/>
+      <c r="AY36" s="56">
+        <v>2</v>
+      </c>
       <c r="AZ36" s="56">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="BA36" s="56"/>
       <c r="BB36">

</xml_diff>

<commit_message>
Trabajo de Fin de Semana
</commit_message>
<xml_diff>
--- a/Finanzas/1_Ene-Feb-Mar_2018.xlsx
+++ b/Finanzas/1_Ene-Feb-Mar_2018.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro\Desktop\Felisa\Finanzas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adriana\Desktop\Felisa\Finanzas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="199">
   <si>
     <t>E L             D I N E R O         E  S             U N             R E C U R S O      L I M I T A D O</t>
   </si>
@@ -606,6 +606,21 @@
   </si>
   <si>
     <t>Dentista Muela 1</t>
+  </si>
+  <si>
+    <t>2 y 7 feb</t>
+  </si>
+  <si>
+    <t>Reparación iPhone</t>
+  </si>
+  <si>
+    <t>Pizzas</t>
+  </si>
+  <si>
+    <t>Visita Abuelita</t>
+  </si>
+  <si>
+    <t>Teatro Enana - Emma</t>
   </si>
 </sst>
 </file>
@@ -1471,8 +1486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BH963"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1751,7 +1766,7 @@
       </c>
       <c r="P4" s="79">
         <f>SUM(N3,R9,P7)</f>
-        <v>41916</v>
+        <v>43346</v>
       </c>
       <c r="Z4" s="47">
         <v>43108</v>
@@ -1930,7 +1945,7 @@
       </c>
       <c r="N6" s="52">
         <f>(SUM((W11:W299),(AC3:AC500),(I11:I499)))-(SUM((X11:X499)))</f>
-        <v>515</v>
+        <v>895</v>
       </c>
       <c r="O6" s="30"/>
       <c r="P6" s="30"/>
@@ -2018,7 +2033,7 @@
       </c>
       <c r="P7" s="78">
         <f>SUM(R7,N6)</f>
-        <v>515</v>
+        <v>895</v>
       </c>
       <c r="Q7" s="75"/>
       <c r="R7" s="74">
@@ -2186,7 +2201,7 @@
       </c>
       <c r="R9" s="15">
         <f>SUM(R11:R481)</f>
-        <v>33290</v>
+        <v>34340</v>
       </c>
       <c r="T9" s="32" t="s">
         <v>40</v>
@@ -3779,10 +3794,18 @@
         <f>P24-Q24</f>
         <v>140</v>
       </c>
-      <c r="T24" s="36"/>
-      <c r="U24" s="35"/>
-      <c r="V24" s="35"/>
-      <c r="W24" s="37"/>
+      <c r="T24" s="36">
+        <v>43141</v>
+      </c>
+      <c r="U24" s="57" t="s">
+        <v>26</v>
+      </c>
+      <c r="V24" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="W24" s="37">
+        <v>450</v>
+      </c>
       <c r="X24" s="37"/>
       <c r="Z24" s="47">
         <v>43128</v>
@@ -4322,11 +4345,11 @@
         <v>2900</v>
       </c>
       <c r="Q30" s="22">
-        <v>500</v>
+        <v>950</v>
       </c>
       <c r="R30" s="20">
         <f t="shared" si="8"/>
-        <v>2400</v>
+        <v>1950</v>
       </c>
       <c r="T30" s="36"/>
       <c r="U30" s="35"/>
@@ -4673,14 +4696,22 @@
       <c r="I34" s="101"/>
       <c r="J34" s="102"/>
       <c r="K34" s="103"/>
-      <c r="M34" s="18"/>
-      <c r="N34" s="18"/>
-      <c r="O34" s="18"/>
-      <c r="P34" s="23"/>
+      <c r="M34" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="N34" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="O34" s="18" t="s">
+        <v>195</v>
+      </c>
+      <c r="P34" s="23">
+        <v>1500</v>
+      </c>
       <c r="Q34" s="22"/>
       <c r="R34" s="20">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1500</v>
       </c>
       <c r="T34" s="36"/>
       <c r="U34" s="35"/>
@@ -4876,7 +4907,7 @@
       </c>
       <c r="AC36" s="41">
         <f t="shared" si="3"/>
-        <v>-432</v>
+        <v>-502</v>
       </c>
       <c r="AD36" s="50">
         <v>80</v>
@@ -4884,9 +4915,14 @@
       <c r="AE36" s="50"/>
       <c r="AG36" s="51">
         <f t="shared" si="0"/>
-        <v>512</v>
-      </c>
-      <c r="AI36" s="56"/>
+        <v>582</v>
+      </c>
+      <c r="AH36">
+        <v>70</v>
+      </c>
+      <c r="AI36" s="56" t="s">
+        <v>196</v>
+      </c>
       <c r="AJ36" s="56" t="s">
         <v>193</v>
       </c>
@@ -4956,7 +4992,9 @@
       <c r="AA37" s="48" t="s">
         <v>70</v>
       </c>
-      <c r="AB37" s="49"/>
+      <c r="AB37" s="49" t="s">
+        <v>197</v>
+      </c>
       <c r="AC37" s="41">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -5027,7 +5065,9 @@
       <c r="AA38" s="48" t="s">
         <v>71</v>
       </c>
-      <c r="AB38" s="49"/>
+      <c r="AB38" s="49" t="s">
+        <v>198</v>
+      </c>
       <c r="AC38" s="41">
         <f t="shared" si="3"/>
         <v>0</v>

</xml_diff>

<commit_message>
Subiendo la Tesis al sistema
</commit_message>
<xml_diff>
--- a/Finanzas/1_Ene-Feb-Mar_2018.xlsx
+++ b/Finanzas/1_Ene-Feb-Mar_2018.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="206">
   <si>
     <t>E L             D I N E R O         E  S             U N             R E C U R S O      L I M I T A D O</t>
   </si>
@@ -621,6 +621,27 @@
   </si>
   <si>
     <t>Teatro Enana - Emma</t>
+  </si>
+  <si>
+    <t>Tramites Titulación</t>
+  </si>
+  <si>
+    <t>Mamá itunes</t>
+  </si>
+  <si>
+    <t>Tacos</t>
+  </si>
+  <si>
+    <t>Nachos y chela</t>
+  </si>
+  <si>
+    <t>Uber Jaime</t>
+  </si>
+  <si>
+    <t>Sushiito</t>
+  </si>
+  <si>
+    <t>Cedula; Título; Fotos; Café internet</t>
   </si>
 </sst>
 </file>
@@ -1486,8 +1507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BH963"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U22" workbookViewId="0">
-      <selection activeCell="AI41" sqref="AI41"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1563,7 +1584,7 @@
       <c r="E2" s="56"/>
       <c r="F2" s="114">
         <f>N3-D2</f>
-        <v>7213</v>
+        <v>4413</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>2</v>
@@ -1690,7 +1711,7 @@
       </c>
       <c r="N3" s="25">
         <f>(SUM(D2,(K11:K499)))-(SUM((J11:J499),(I11:I499)))</f>
-        <v>8111</v>
+        <v>5311</v>
       </c>
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
@@ -1766,7 +1787,7 @@
       </c>
       <c r="P4" s="79">
         <f>SUM(N3,R9,P7)</f>
-        <v>43482</v>
+        <v>40390</v>
       </c>
       <c r="Z4" s="47">
         <v>43108</v>
@@ -1945,7 +1966,7 @@
       </c>
       <c r="N6" s="52">
         <f>(SUM((W11:W299),(AC3:AC500),(I11:I499)))-(SUM((X11:X499)))</f>
-        <v>1031</v>
+        <v>739</v>
       </c>
       <c r="O6" s="30"/>
       <c r="P6" s="30"/>
@@ -2033,7 +2054,7 @@
       </c>
       <c r="P7" s="78">
         <f>SUM(R7,N6)</f>
-        <v>1031</v>
+        <v>739</v>
       </c>
       <c r="Q7" s="75"/>
       <c r="R7" s="74">
@@ -3095,9 +3116,13 @@
         <v>0</v>
       </c>
       <c r="G17" s="99"/>
-      <c r="H17" s="56"/>
+      <c r="H17" s="56" t="s">
+        <v>200</v>
+      </c>
       <c r="I17" s="104"/>
-      <c r="J17" s="102"/>
+      <c r="J17" s="102">
+        <v>300</v>
+      </c>
       <c r="K17" s="103"/>
       <c r="M17" s="18"/>
       <c r="N17" s="18" t="s">
@@ -3183,9 +3208,15 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="G18" s="99"/>
-      <c r="H18" s="56"/>
-      <c r="I18" s="101"/>
+      <c r="G18" s="99">
+        <v>43150</v>
+      </c>
+      <c r="H18" s="56" t="s">
+        <v>199</v>
+      </c>
+      <c r="I18" s="101">
+        <v>2500</v>
+      </c>
       <c r="J18" s="102"/>
       <c r="K18" s="103"/>
       <c r="M18" s="18"/>
@@ -5324,7 +5355,9 @@
       <c r="AH41">
         <v>150</v>
       </c>
-      <c r="AI41" s="56"/>
+      <c r="AI41" s="56" t="s">
+        <v>204</v>
+      </c>
       <c r="AJ41" s="56"/>
       <c r="AK41" s="56"/>
       <c r="AL41" s="56"/>
@@ -5405,7 +5438,9 @@
       <c r="AH42">
         <v>70</v>
       </c>
-      <c r="AI42" s="56"/>
+      <c r="AI42" s="56" t="s">
+        <v>114</v>
+      </c>
       <c r="AJ42" s="56"/>
       <c r="AK42" s="56"/>
       <c r="AL42" s="56"/>
@@ -5473,7 +5508,7 @@
       <c r="AB43" s="49"/>
       <c r="AC43" s="41">
         <f t="shared" si="3"/>
-        <v>80</v>
+        <v>14</v>
       </c>
       <c r="AD43" s="50">
         <v>80</v>
@@ -5481,11 +5516,20 @@
       <c r="AE43" s="50"/>
       <c r="AG43" s="51">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AI43" s="56"/>
-      <c r="AJ43" s="56"/>
-      <c r="AK43" s="56"/>
+        <v>66</v>
+      </c>
+      <c r="AH43">
+        <v>40</v>
+      </c>
+      <c r="AI43" s="56" t="s">
+        <v>201</v>
+      </c>
+      <c r="AJ43" s="56" t="s">
+        <v>202</v>
+      </c>
+      <c r="AK43" s="56">
+        <v>20</v>
+      </c>
       <c r="AL43" s="56"/>
       <c r="AM43" s="56"/>
       <c r="AN43" s="56"/>
@@ -5497,7 +5541,7 @@
       <c r="AT43" s="56"/>
       <c r="AU43">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AV43" s="102"/>
       <c r="AW43" s="56"/>
@@ -5511,6 +5555,9 @@
       <c r="BB43">
         <f t="shared" si="4"/>
         <v>0</v>
+      </c>
+      <c r="BC43">
+        <v>6</v>
       </c>
     </row>
     <row r="44" spans="5:56" x14ac:dyDescent="0.25">
@@ -5546,17 +5593,28 @@
       <c r="AB44" s="72"/>
       <c r="AC44" s="41">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AD44" s="50"/>
+        <v>-105</v>
+      </c>
+      <c r="AD44" s="50">
+        <v>100</v>
+      </c>
       <c r="AE44" s="50"/>
       <c r="AG44" s="51">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AI44" s="100"/>
-      <c r="AJ44" s="56"/>
-      <c r="AK44" s="56"/>
+        <v>205</v>
+      </c>
+      <c r="AH44">
+        <v>100</v>
+      </c>
+      <c r="AI44" s="100" t="s">
+        <v>152</v>
+      </c>
+      <c r="AJ44" s="56" t="s">
+        <v>203</v>
+      </c>
+      <c r="AK44" s="56">
+        <v>100</v>
+      </c>
       <c r="AL44" s="56"/>
       <c r="AM44" s="56"/>
       <c r="AN44" s="56"/>
@@ -5568,7 +5626,7 @@
       <c r="AT44" s="56"/>
       <c r="AU44">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AV44" s="102"/>
       <c r="AW44" s="102"/>
@@ -5578,10 +5636,12 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="BA44" s="56"/>
+      <c r="BA44" s="56">
+        <v>1</v>
+      </c>
       <c r="BB44">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="45" spans="5:56" x14ac:dyDescent="0.25">
@@ -5689,20 +5749,37 @@
       <c r="AB46" s="49"/>
       <c r="AC46" s="41">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AD46" s="50"/>
+        <v>-2621</v>
+      </c>
+      <c r="AD46" s="50">
+        <v>120</v>
+      </c>
       <c r="AE46" s="50"/>
       <c r="AG46" s="51">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AI46" s="100"/>
-      <c r="AJ46" s="56"/>
-      <c r="AK46" s="56"/>
-      <c r="AL46" s="56"/>
-      <c r="AM46" s="56"/>
-      <c r="AN46" s="56"/>
+        <v>2741</v>
+      </c>
+      <c r="AH46">
+        <v>70</v>
+      </c>
+      <c r="AI46" s="100" t="s">
+        <v>155</v>
+      </c>
+      <c r="AJ46" s="100" t="s">
+        <v>205</v>
+      </c>
+      <c r="AK46" s="56">
+        <v>1261</v>
+      </c>
+      <c r="AL46" s="56">
+        <v>1000</v>
+      </c>
+      <c r="AM46" s="56">
+        <v>385</v>
+      </c>
+      <c r="AN46" s="56">
+        <v>15</v>
+      </c>
       <c r="AO46" s="56"/>
       <c r="AP46" s="56"/>
       <c r="AQ46" s="56"/>
@@ -5711,7 +5788,7 @@
       <c r="AT46" s="56"/>
       <c r="AU46">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AV46" s="56"/>
       <c r="AW46" s="56"/>
@@ -5721,10 +5798,12 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="BA46" s="56"/>
+      <c r="BA46" s="56">
+        <v>2</v>
+      </c>
       <c r="BB46">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="47" spans="5:56" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Creando version a imprimir de la Tesis
</commit_message>
<xml_diff>
--- a/Finanzas/1_Ene-Feb-Mar_2018.xlsx
+++ b/Finanzas/1_Ene-Feb-Mar_2018.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adriana\Desktop\Felisa\Finanzas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro\Desktop\Felisa\Finanzas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="231">
   <si>
     <t>E L             D I N E R O         E  S             U N             R E C U R S O      L I M I T A D O</t>
   </si>
@@ -705,6 +705,18 @@
   </si>
   <si>
     <t>Crepas</t>
+  </si>
+  <si>
+    <t>Descanso Fiebre</t>
+  </si>
+  <si>
+    <t>Valoración Nariz</t>
+  </si>
+  <si>
+    <t>No comí</t>
+  </si>
+  <si>
+    <t>Comí casa</t>
   </si>
 </sst>
 </file>
@@ -1570,9 +1582,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BH963"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="U18" sqref="U18"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1850,7 +1860,7 @@
       </c>
       <c r="P4" s="79">
         <f>SUM(N3,R9,P7)</f>
-        <v>41177</v>
+        <v>41364</v>
       </c>
       <c r="Z4" s="47">
         <v>43108</v>
@@ -1923,7 +1933,7 @@
       </c>
       <c r="BG4" s="57">
         <f>(SUM((AV3:AV519)))-(SUM((AZ3:AZ519)))</f>
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="BH4" s="57"/>
     </row>
@@ -2029,7 +2039,7 @@
       </c>
       <c r="N6" s="52">
         <f>(SUM((W11:W299),(AC3:AC500),(I11:I499)))-(SUM((X11:X499)))</f>
-        <v>2126</v>
+        <v>2313</v>
       </c>
       <c r="O6" s="30"/>
       <c r="P6" s="30"/>
@@ -2117,7 +2127,7 @@
       </c>
       <c r="P7" s="78">
         <f>SUM(R7,N6)</f>
-        <v>2126</v>
+        <v>2313</v>
       </c>
       <c r="Q7" s="75"/>
       <c r="R7" s="74">
@@ -6396,7 +6406,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AI52" s="56"/>
+      <c r="AH52">
+        <v>0</v>
+      </c>
+      <c r="AI52" s="56" t="s">
+        <v>99</v>
+      </c>
       <c r="AJ52" s="56"/>
       <c r="AK52" s="56"/>
       <c r="AL52" s="56"/>
@@ -6454,20 +6469,33 @@
       <c r="AA53" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="AB53" s="49"/>
+      <c r="AB53" s="49" t="s">
+        <v>227</v>
+      </c>
       <c r="AC53" s="41">
         <f t="shared" si="3"/>
-        <v>-50</v>
-      </c>
-      <c r="AD53" s="50"/>
+        <v>57</v>
+      </c>
+      <c r="AD53" s="50">
+        <v>120</v>
+      </c>
       <c r="AE53" s="50"/>
       <c r="AG53" s="51">
         <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="AI53" s="56"/>
-      <c r="AJ53" s="56"/>
-      <c r="AK53" s="56"/>
+        <v>63</v>
+      </c>
+      <c r="AH53">
+        <v>0</v>
+      </c>
+      <c r="AI53" s="56" t="s">
+        <v>230</v>
+      </c>
+      <c r="AJ53" s="56" t="s">
+        <v>112</v>
+      </c>
+      <c r="AK53" s="56">
+        <v>13</v>
+      </c>
       <c r="AL53" s="56"/>
       <c r="AM53" s="102"/>
       <c r="AN53" s="56"/>
@@ -6527,18 +6555,27 @@
       <c r="AA54" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="AB54" s="49"/>
+      <c r="AB54" s="49" t="s">
+        <v>228</v>
+      </c>
       <c r="AC54" s="41">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AD54" s="50"/>
+        <v>80</v>
+      </c>
+      <c r="AD54" s="50">
+        <v>80</v>
+      </c>
       <c r="AE54" s="85"/>
       <c r="AG54" s="51">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AI54" s="56"/>
+      <c r="AH54">
+        <v>0</v>
+      </c>
+      <c r="AI54" s="56" t="s">
+        <v>229</v>
+      </c>
       <c r="AJ54" s="56"/>
       <c r="AK54" s="56"/>
       <c r="AL54" s="56"/>
@@ -6555,12 +6592,16 @@
         <v>0</v>
       </c>
       <c r="AV54" s="56"/>
-      <c r="AW54" s="56"/>
+      <c r="AW54" s="56">
+        <v>2</v>
+      </c>
       <c r="AX54" s="56"/>
-      <c r="AY54" s="56"/>
+      <c r="AY54" s="56">
+        <v>1</v>
+      </c>
       <c r="AZ54" s="56">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="BA54" s="56"/>
       <c r="BB54">

</xml_diff>

<commit_message>
Lista para imprimir casi
</commit_message>
<xml_diff>
--- a/Finanzas/1_Ene-Feb-Mar_2018.xlsx
+++ b/Finanzas/1_Ene-Feb-Mar_2018.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="233">
   <si>
     <t>E L             D I N E R O         E  S             U N             R E C U R S O      L I M I T A D O</t>
   </si>
@@ -717,6 +717,12 @@
   </si>
   <si>
     <t>Comí casa</t>
+  </si>
+  <si>
+    <t>Otra vez no cine con Angel</t>
+  </si>
+  <si>
+    <t>Coca</t>
   </si>
 </sst>
 </file>
@@ -1582,7 +1588,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BH963"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="T34" workbookViewId="0">
+      <selection activeCell="AB55" sqref="AB55"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1860,7 +1868,7 @@
       </c>
       <c r="P4" s="79">
         <f>SUM(N3,R9,P7)</f>
-        <v>41364</v>
+        <v>41341</v>
       </c>
       <c r="Z4" s="47">
         <v>43108</v>
@@ -1933,7 +1941,7 @@
       </c>
       <c r="BG4" s="57">
         <f>(SUM((AV3:AV519)))-(SUM((AZ3:AZ519)))</f>
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="BH4" s="57"/>
     </row>
@@ -2039,7 +2047,7 @@
       </c>
       <c r="N6" s="52">
         <f>(SUM((W11:W299),(AC3:AC500),(I11:I499)))-(SUM((X11:X499)))</f>
-        <v>2313</v>
+        <v>2290</v>
       </c>
       <c r="O6" s="30"/>
       <c r="P6" s="30"/>
@@ -2127,7 +2135,7 @@
       </c>
       <c r="P7" s="78">
         <f>SUM(R7,N6)</f>
-        <v>2313</v>
+        <v>2290</v>
       </c>
       <c r="Q7" s="75"/>
       <c r="R7" s="74">
@@ -6560,7 +6568,7 @@
       </c>
       <c r="AC54" s="41">
         <f t="shared" si="3"/>
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="AD54" s="50">
         <v>80</v>
@@ -6568,7 +6576,7 @@
       <c r="AE54" s="85"/>
       <c r="AG54" s="51">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="AH54">
         <v>0</v>
@@ -6576,8 +6584,12 @@
       <c r="AI54" s="56" t="s">
         <v>229</v>
       </c>
-      <c r="AJ54" s="56"/>
-      <c r="AK54" s="56"/>
+      <c r="AJ54" s="56" t="s">
+        <v>232</v>
+      </c>
+      <c r="AK54" s="56">
+        <v>14</v>
+      </c>
       <c r="AL54" s="56"/>
       <c r="AM54" s="56"/>
       <c r="AN54" s="56"/>
@@ -6597,11 +6609,11 @@
       </c>
       <c r="AX54" s="56"/>
       <c r="AY54" s="56">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AZ54" s="56">
         <f t="shared" si="7"/>
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="BA54" s="56"/>
       <c r="BB54">
@@ -6637,20 +6649,33 @@
       <c r="AA55" s="48" t="s">
         <v>73</v>
       </c>
-      <c r="AB55" s="49"/>
+      <c r="AB55" s="49" t="s">
+        <v>231</v>
+      </c>
       <c r="AC55" s="41">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AD55" s="50"/>
+        <v>-9</v>
+      </c>
+      <c r="AD55" s="50">
+        <v>100</v>
+      </c>
       <c r="AE55" s="50"/>
       <c r="AG55" s="51">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AI55" s="56"/>
-      <c r="AJ55" s="56"/>
-      <c r="AK55" s="56"/>
+        <v>109</v>
+      </c>
+      <c r="AH55">
+        <v>75</v>
+      </c>
+      <c r="AI55" s="56" t="s">
+        <v>191</v>
+      </c>
+      <c r="AJ55" s="56" t="s">
+        <v>232</v>
+      </c>
+      <c r="AK55" s="56">
+        <v>18</v>
+      </c>
       <c r="AL55" s="56"/>
       <c r="AM55" s="56"/>
       <c r="AN55" s="56"/>
@@ -6662,7 +6687,7 @@
       <c r="AT55" s="56"/>
       <c r="AU55">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AV55" s="56"/>
       <c r="AW55" s="56"/>
@@ -6672,10 +6697,15 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="BA55" s="56"/>
+      <c r="BA55" s="56">
+        <v>2</v>
+      </c>
       <c r="BB55">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="BC55">
+        <v>6</v>
       </c>
     </row>
     <row r="56" spans="5:55" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Modelo de diferencias en Tau
</commit_message>
<xml_diff>
--- a/Finanzas/1_Ene-Feb-Mar_2018.xlsx
+++ b/Finanzas/1_Ene-Feb-Mar_2018.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adriana\Desktop\Felisa\Finanzas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro\Desktop\Felisa\Finanzas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="253">
   <si>
     <t>E L             D I N E R O         E  S             U N             R E C U R S O      L I M I T A D O</t>
   </si>
@@ -744,6 +744,45 @@
   </si>
   <si>
     <t>Chocolate y Cerveza</t>
+  </si>
+  <si>
+    <t>Jaime me dio 250</t>
+  </si>
+  <si>
+    <t>Casa de Toño</t>
+  </si>
+  <si>
+    <t>Jaime me dio para alcohol</t>
+  </si>
+  <si>
+    <t>Taquitos</t>
+  </si>
+  <si>
+    <t>Michael Day 1</t>
+  </si>
+  <si>
+    <t>Michael Day 2</t>
+  </si>
+  <si>
+    <t>CUMPLE :D</t>
+  </si>
+  <si>
+    <t>Michael Day 4</t>
+  </si>
+  <si>
+    <t>Enana Minecraft</t>
+  </si>
+  <si>
+    <t>Enana</t>
+  </si>
+  <si>
+    <t>Minecraft</t>
+  </si>
+  <si>
+    <t>Juego Da Vinci</t>
+  </si>
+  <si>
+    <t>Azucar</t>
   </si>
 </sst>
 </file>
@@ -1609,8 +1648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BH963"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z45" workbookViewId="0">
-      <selection activeCell="AJ56" sqref="AJ56"/>
+    <sheetView tabSelected="1" topLeftCell="V34" workbookViewId="0">
+      <selection activeCell="AO57" sqref="AO57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1686,7 +1725,7 @@
       <c r="E2" s="56"/>
       <c r="F2" s="114">
         <f>N3-D2</f>
-        <v>4413</v>
+        <v>4083</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>2</v>
@@ -1813,7 +1852,7 @@
       </c>
       <c r="N3" s="25">
         <f>(SUM(D2,(K11:K499)))-(SUM((J11:J499),(I11:I499)))</f>
-        <v>5311</v>
+        <v>4981</v>
       </c>
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
@@ -1889,7 +1928,7 @@
       </c>
       <c r="P4" s="79">
         <f>SUM(N3,R9,P7)</f>
-        <v>41751</v>
+        <v>41588</v>
       </c>
       <c r="Z4" s="47">
         <v>43108</v>
@@ -2068,7 +2107,7 @@
       </c>
       <c r="N6" s="52">
         <f>(SUM((W11:W299),(AC3:AC500),(I11:I499)))-(SUM((X11:X499)))</f>
-        <v>2700</v>
+        <v>2637</v>
       </c>
       <c r="O6" s="30"/>
       <c r="P6" s="30"/>
@@ -2156,7 +2195,7 @@
       </c>
       <c r="P7" s="78">
         <f>SUM(R7,N6)</f>
-        <v>2700</v>
+        <v>2637</v>
       </c>
       <c r="Q7" s="75"/>
       <c r="R7" s="74">
@@ -2324,7 +2363,7 @@
       </c>
       <c r="R9" s="15">
         <f>SUM(R11:R481)</f>
-        <v>33740</v>
+        <v>33970</v>
       </c>
       <c r="T9" s="32" t="s">
         <v>40</v>
@@ -3420,9 +3459,13 @@
         <v>0</v>
       </c>
       <c r="G19" s="99"/>
-      <c r="H19" s="56"/>
+      <c r="H19" s="56" t="s">
+        <v>248</v>
+      </c>
       <c r="I19" s="101"/>
-      <c r="J19" s="102"/>
+      <c r="J19" s="102">
+        <v>130</v>
+      </c>
       <c r="K19" s="103"/>
       <c r="M19" s="18"/>
       <c r="N19" s="18" t="s">
@@ -3506,9 +3549,13 @@
         <v>0</v>
       </c>
       <c r="G20" s="99"/>
-      <c r="H20" s="56"/>
+      <c r="H20" s="56" t="s">
+        <v>123</v>
+      </c>
       <c r="I20" s="101"/>
-      <c r="J20" s="102"/>
+      <c r="J20" s="102">
+        <v>200</v>
+      </c>
       <c r="K20" s="103"/>
       <c r="M20" s="18"/>
       <c r="N20" s="18" t="s">
@@ -4967,13 +5014,19 @@
       <c r="J35" s="102"/>
       <c r="K35" s="103"/>
       <c r="M35" s="18"/>
-      <c r="N35" s="18"/>
-      <c r="O35" s="18"/>
-      <c r="P35" s="23"/>
+      <c r="N35" s="18" t="s">
+        <v>249</v>
+      </c>
+      <c r="O35" s="18" t="s">
+        <v>250</v>
+      </c>
+      <c r="P35" s="23">
+        <v>130</v>
+      </c>
       <c r="Q35" s="22"/>
       <c r="R35" s="20">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>130</v>
       </c>
       <c r="T35" s="36"/>
       <c r="U35" s="35"/>
@@ -5052,13 +5105,19 @@
       <c r="J36" s="102"/>
       <c r="K36" s="103"/>
       <c r="M36" s="18"/>
-      <c r="N36" s="18"/>
-      <c r="O36" s="18"/>
-      <c r="P36" s="23"/>
+      <c r="N36" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="O36" s="18" t="s">
+        <v>251</v>
+      </c>
+      <c r="P36" s="23">
+        <v>100</v>
+      </c>
       <c r="Q36" s="22"/>
       <c r="R36" s="20">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="T36" s="36"/>
       <c r="U36" s="35"/>
@@ -6770,7 +6829,7 @@
       </c>
       <c r="AC56" s="41">
         <f t="shared" si="3"/>
-        <v>-1447</v>
+        <v>-1475</v>
       </c>
       <c r="AD56" s="50">
         <v>80</v>
@@ -6778,7 +6837,7 @@
       <c r="AE56" s="50"/>
       <c r="AG56" s="51">
         <f t="shared" si="0"/>
-        <v>1527</v>
+        <v>1555</v>
       </c>
       <c r="AH56">
         <v>0</v>
@@ -6786,11 +6845,15 @@
       <c r="AI56" s="56" t="s">
         <v>201</v>
       </c>
-      <c r="AJ56" s="56"/>
+      <c r="AJ56" s="56" t="s">
+        <v>154</v>
+      </c>
       <c r="AK56" s="102">
         <v>1500</v>
       </c>
-      <c r="AL56" s="56"/>
+      <c r="AL56" s="56">
+        <v>28</v>
+      </c>
       <c r="AM56" s="56"/>
       <c r="AN56" s="56"/>
       <c r="AO56" s="56"/>
@@ -7098,18 +7161,32 @@
       <c r="AA60" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="AB60" s="49"/>
+      <c r="AB60" s="49" t="s">
+        <v>244</v>
+      </c>
       <c r="AC60" s="41">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AD60" s="50"/>
-      <c r="AE60" s="50"/>
+        <v>289</v>
+      </c>
+      <c r="AD60" s="50">
+        <v>120</v>
+      </c>
+      <c r="AE60" s="50">
+        <v>250</v>
+      </c>
+      <c r="AF60" t="s">
+        <v>240</v>
+      </c>
       <c r="AG60" s="51">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AI60" s="56"/>
+        <v>81</v>
+      </c>
+      <c r="AH60">
+        <v>70</v>
+      </c>
+      <c r="AI60" s="56" t="s">
+        <v>155</v>
+      </c>
       <c r="AJ60" s="56"/>
       <c r="AK60" s="56"/>
       <c r="AL60" s="56"/>
@@ -7123,7 +7200,7 @@
       <c r="AT60" s="56"/>
       <c r="AU60">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="AV60" s="56"/>
       <c r="AW60" s="56"/>
@@ -7133,10 +7210,15 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="BA60" s="56"/>
+      <c r="BA60" s="56">
+        <v>0</v>
+      </c>
       <c r="BB60">
         <f t="shared" si="4"/>
         <v>0</v>
+      </c>
+      <c r="BC60">
+        <v>11</v>
       </c>
     </row>
     <row r="61" spans="5:55" x14ac:dyDescent="0.25">
@@ -7167,21 +7249,39 @@
       <c r="AA61" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="AB61" s="49"/>
+      <c r="AB61" s="49" t="s">
+        <v>245</v>
+      </c>
       <c r="AC61" s="41">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AD61" s="50"/>
-      <c r="AE61" s="50"/>
+        <v>-430</v>
+      </c>
+      <c r="AD61" s="50">
+        <v>80</v>
+      </c>
+      <c r="AE61" s="50">
+        <v>100</v>
+      </c>
+      <c r="AF61" t="s">
+        <v>242</v>
+      </c>
       <c r="AG61" s="51">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AI61" s="56"/>
+        <v>610</v>
+      </c>
+      <c r="AH61">
+        <v>146</v>
+      </c>
+      <c r="AI61" s="56" t="s">
+        <v>241</v>
+      </c>
       <c r="AJ61" s="56"/>
-      <c r="AK61" s="56"/>
-      <c r="AL61" s="56"/>
+      <c r="AK61" s="56">
+        <v>28</v>
+      </c>
+      <c r="AL61" s="56">
+        <v>420</v>
+      </c>
       <c r="AM61" s="56"/>
       <c r="AN61" s="56"/>
       <c r="AO61" s="56"/>
@@ -7192,7 +7292,7 @@
       <c r="AT61" s="56"/>
       <c r="AU61">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AV61" s="56"/>
       <c r="AW61" s="56"/>
@@ -7202,10 +7302,15 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="BA61" s="56"/>
+      <c r="BA61" s="56">
+        <v>2</v>
+      </c>
       <c r="BB61">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="BC61">
+        <v>6</v>
       </c>
     </row>
     <row r="62" spans="5:55" x14ac:dyDescent="0.25">
@@ -7236,21 +7341,34 @@
       <c r="AA62" s="48" t="s">
         <v>73</v>
       </c>
-      <c r="AB62" s="49"/>
+      <c r="AB62" s="49" t="s">
+        <v>246</v>
+      </c>
       <c r="AC62" s="41">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AD62" s="50"/>
+        <v>26</v>
+      </c>
+      <c r="AD62" s="50">
+        <v>80</v>
+      </c>
       <c r="AE62" s="50"/>
       <c r="AG62" s="51">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AI62" s="56"/>
-      <c r="AJ62" s="56"/>
-      <c r="AK62" s="56"/>
-      <c r="AL62" s="102"/>
+        <v>54</v>
+      </c>
+      <c r="AH62">
+        <v>20</v>
+      </c>
+      <c r="AI62" s="56" t="s">
+        <v>243</v>
+      </c>
+      <c r="AJ62" s="56" t="s">
+        <v>252</v>
+      </c>
+      <c r="AK62" s="56">
+        <v>23</v>
+      </c>
+      <c r="AL62" s="95"/>
       <c r="AM62" s="56"/>
       <c r="AN62" s="56"/>
       <c r="AO62" s="56"/>
@@ -7261,7 +7379,7 @@
       <c r="AT62" s="56"/>
       <c r="AU62">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="AV62" s="56"/>
       <c r="AW62" s="56"/>
@@ -7271,10 +7389,15 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="BA62" s="56"/>
+      <c r="BA62" s="56">
+        <v>1</v>
+      </c>
       <c r="BB62">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="BC62">
+        <v>6</v>
       </c>
     </row>
     <row r="63" spans="5:55" x14ac:dyDescent="0.25">
@@ -7305,12 +7428,16 @@
       <c r="AA63" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="AB63" s="49"/>
+      <c r="AB63" s="49" t="s">
+        <v>247</v>
+      </c>
       <c r="AC63" s="41">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AD63" s="50"/>
+        <v>80</v>
+      </c>
+      <c r="AD63" s="50">
+        <v>80</v>
+      </c>
       <c r="AE63" s="50"/>
       <c r="AG63" s="51">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Los histogramas no están normalizados
</commit_message>
<xml_diff>
--- a/Finanzas/1_Ene-Feb-Mar_2018.xlsx
+++ b/Finanzas/1_Ene-Feb-Mar_2018.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="255">
   <si>
     <t>E L             D I N E R O         E  S             U N             R E C U R S O      L I M I T A D O</t>
   </si>
@@ -783,6 +783,12 @@
   </si>
   <si>
     <t>Azucar</t>
+  </si>
+  <si>
+    <t>Taxi</t>
+  </si>
+  <si>
+    <t>Doña Lulá</t>
   </si>
 </sst>
 </file>
@@ -1648,8 +1654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BH963"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V34" workbookViewId="0">
-      <selection activeCell="AO57" sqref="AO57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1928,7 +1934,7 @@
       </c>
       <c r="P4" s="79">
         <f>SUM(N3,R9,P7)</f>
-        <v>41588</v>
+        <v>41434</v>
       </c>
       <c r="Z4" s="47">
         <v>43108</v>
@@ -2107,7 +2113,7 @@
       </c>
       <c r="N6" s="52">
         <f>(SUM((W11:W299),(AC3:AC500),(I11:I499)))-(SUM((X11:X499)))</f>
-        <v>2637</v>
+        <v>2483</v>
       </c>
       <c r="O6" s="30"/>
       <c r="P6" s="30"/>
@@ -2195,7 +2201,7 @@
       </c>
       <c r="P7" s="78">
         <f>SUM(R7,N6)</f>
-        <v>2637</v>
+        <v>2483</v>
       </c>
       <c r="Q7" s="75"/>
       <c r="R7" s="74">
@@ -7433,19 +7439,28 @@
       </c>
       <c r="AC63" s="41">
         <f t="shared" si="3"/>
-        <v>80</v>
+        <v>-74</v>
       </c>
       <c r="AD63" s="50">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="AE63" s="50"/>
       <c r="AG63" s="51">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AI63" s="56"/>
-      <c r="AJ63" s="56"/>
-      <c r="AK63" s="56"/>
+        <v>194</v>
+      </c>
+      <c r="AH63">
+        <v>155</v>
+      </c>
+      <c r="AI63" s="56" t="s">
+        <v>254</v>
+      </c>
+      <c r="AJ63" s="56" t="s">
+        <v>253</v>
+      </c>
+      <c r="AK63" s="56">
+        <v>15</v>
+      </c>
       <c r="AL63" s="56"/>
       <c r="AM63" s="56"/>
       <c r="AN63" s="56"/>
@@ -7457,7 +7472,7 @@
       <c r="AT63" s="56"/>
       <c r="AU63">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="AV63" s="56"/>
       <c r="AW63" s="56"/>
@@ -7467,10 +7482,15 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="BA63" s="56"/>
+      <c r="BA63" s="56">
+        <v>2</v>
+      </c>
       <c r="BB63">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="BC63">
+        <v>14</v>
       </c>
     </row>
     <row r="64" spans="5:55" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Acomodando carpetas de ingles
</commit_message>
<xml_diff>
--- a/Finanzas/1_Ene-Feb-Mar_2018.xlsx
+++ b/Finanzas/1_Ene-Feb-Mar_2018.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="283">
   <si>
     <t>E L             D I N E R O         E  S             U N             R E C U R S O      L I M I T A D O</t>
   </si>
@@ -853,6 +853,21 @@
   </si>
   <si>
     <t>Estudios Sangre</t>
+  </si>
+  <si>
+    <t>Sol comida</t>
+  </si>
+  <si>
+    <t>Ale problemas</t>
+  </si>
+  <si>
+    <t>Seminario Stephane</t>
+  </si>
+  <si>
+    <t>Arquitectura</t>
+  </si>
+  <si>
+    <t>Pantalones Sol</t>
   </si>
 </sst>
 </file>
@@ -1708,7 +1723,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1718,8 +1733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BH963"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L13" workbookViewId="0">
-      <selection activeCell="V33" sqref="V33"/>
+    <sheetView tabSelected="1" topLeftCell="AL53" workbookViewId="0">
+      <selection activeCell="AY77" sqref="AY77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1998,7 +2013,7 @@
       </c>
       <c r="P4" s="79">
         <f>SUM(N3,R9,P7)</f>
-        <v>40796</v>
+        <v>40920</v>
       </c>
       <c r="Z4" s="47">
         <v>43108</v>
@@ -2071,7 +2086,7 @@
       </c>
       <c r="BG4" s="57">
         <f>(SUM((AV3:AV519)))-(SUM((AZ3:AZ519)))</f>
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="BH4" s="57"/>
     </row>
@@ -2177,7 +2192,7 @@
       </c>
       <c r="N6" s="52">
         <f>(SUM((W11:W299),(AC3:AC500),(I11:I499)))-(SUM((X11:X499)))</f>
-        <v>1945</v>
+        <v>2069</v>
       </c>
       <c r="O6" s="30"/>
       <c r="P6" s="30"/>
@@ -2265,7 +2280,7 @@
       </c>
       <c r="P7" s="78">
         <f>SUM(R7,N6)</f>
-        <v>1945</v>
+        <v>2069</v>
       </c>
       <c r="Q7" s="75"/>
       <c r="R7" s="74">
@@ -4748,7 +4763,7 @@
       </c>
       <c r="V31" s="35"/>
       <c r="W31" s="37">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="X31" s="37"/>
       <c r="Z31" s="47">
@@ -4833,7 +4848,7 @@
       </c>
       <c r="V32" s="35"/>
       <c r="W32" s="37">
-        <v>100</v>
+        <v>250</v>
       </c>
       <c r="X32" s="37"/>
       <c r="Z32" s="47">
@@ -8613,20 +8628,33 @@
       <c r="AA76" s="48" t="s">
         <v>73</v>
       </c>
-      <c r="AB76" s="49"/>
+      <c r="AB76" s="49" t="s">
+        <v>278</v>
+      </c>
       <c r="AC76" s="41">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AD76" s="50"/>
+        <v>-184</v>
+      </c>
+      <c r="AD76" s="50">
+        <v>80</v>
+      </c>
       <c r="AE76" s="50"/>
       <c r="AG76" s="51">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AI76" s="56"/>
-      <c r="AJ76" s="56"/>
-      <c r="AK76" s="56"/>
+        <v>264</v>
+      </c>
+      <c r="AH76">
+        <v>64</v>
+      </c>
+      <c r="AI76" s="56" t="s">
+        <v>281</v>
+      </c>
+      <c r="AJ76" s="56" t="s">
+        <v>282</v>
+      </c>
+      <c r="AK76" s="56">
+        <v>200</v>
+      </c>
       <c r="AL76" s="56"/>
       <c r="AM76" s="56"/>
       <c r="AN76" s="56"/>
@@ -8682,18 +8710,27 @@
       <c r="AA77" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="AB77" s="49"/>
+      <c r="AB77" s="49" t="s">
+        <v>279</v>
+      </c>
       <c r="AC77" s="41">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AD77" s="50"/>
+        <v>-22</v>
+      </c>
+      <c r="AD77" s="50">
+        <v>80</v>
+      </c>
       <c r="AE77" s="50"/>
       <c r="AG77" s="51">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AI77" s="56"/>
+        <v>102</v>
+      </c>
+      <c r="AH77">
+        <v>70</v>
+      </c>
+      <c r="AI77" s="56" t="s">
+        <v>114</v>
+      </c>
       <c r="AJ77" s="56"/>
       <c r="AK77" s="56"/>
       <c r="AL77" s="56"/>
@@ -8707,20 +8744,29 @@
       <c r="AT77" s="56"/>
       <c r="AU77">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AV77" s="56"/>
-      <c r="AW77" s="56"/>
+        <v>32</v>
+      </c>
+      <c r="AV77" s="56">
+        <v>15</v>
+      </c>
+      <c r="AW77" s="56">
+        <v>2</v>
+      </c>
       <c r="AX77" s="56"/>
-      <c r="AY77" s="56"/>
+      <c r="AY77" s="56">
+        <v>2</v>
+      </c>
       <c r="AZ77" s="56">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="BA77" s="56"/>
       <c r="BB77">
         <f t="shared" si="13"/>
         <v>0</v>
+      </c>
+      <c r="BC77">
+        <v>17</v>
       </c>
     </row>
     <row r="78" spans="5:55" x14ac:dyDescent="0.25">
@@ -8751,12 +8797,16 @@
       <c r="AA78" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="AB78" s="49"/>
+      <c r="AB78" s="49" t="s">
+        <v>280</v>
+      </c>
       <c r="AC78" s="41">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AD78" s="50"/>
+        <v>80</v>
+      </c>
+      <c r="AD78" s="50">
+        <v>80</v>
+      </c>
       <c r="AE78" s="50"/>
       <c r="AG78" s="51">
         <f t="shared" si="10"/>

</xml_diff>